<commit_message>
11:54 time 24.10.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -1,92 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asosiy\Teloegram_bot_P\Nodavlat_MTT\file_service\file_database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910B329A-D6A4-4E3F-9256-81A5F074AA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>F.I.SH</t>
-  </si>
-  <si>
-    <t>Ta'lim yo'nalishi</t>
-  </si>
-  <si>
-    <t>Passport</t>
-  </si>
-  <si>
-    <t>Shartnoma raqam</t>
-  </si>
-  <si>
-    <t>Viloyat</t>
-  </si>
-  <si>
-    <t>Tuman</t>
-  </si>
-  <si>
-    <t>Telefon raqam</t>
-  </si>
-  <si>
-    <t>Sana</t>
-  </si>
-  <si>
-    <t>Amirov Akrom Eshali o'g'li</t>
-  </si>
-  <si>
-    <t>Maktabgacha ta’lim tashkiloti tarbiyachisi</t>
-  </si>
-  <si>
-    <t>AC9990099</t>
-  </si>
-  <si>
-    <t>171</t>
-  </si>
-  <si>
-    <t>Namangan viloyati</t>
-  </si>
-  <si>
-    <t>Toʻraqoʻrgʻon tumani</t>
-  </si>
-  <si>
-    <t>+998945289910</t>
-  </si>
-  <si>
-    <t>06-10-2024</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -120,30 +62,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -443,75 +444,195 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col width="42.85546875" customWidth="1" min="1" max="1"/>
+    <col width="58.7109375" customWidth="1" min="2" max="2"/>
+    <col width="16.85546875" customWidth="1" min="3" max="3"/>
+    <col width="10.42578125" customWidth="1" min="4" max="4"/>
+    <col width="45.85546875" customWidth="1" min="5" max="5"/>
+    <col width="41" customWidth="1" min="6" max="6"/>
+    <col width="18.28515625" customWidth="1" min="7" max="7"/>
+    <col width="18.140625" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
+    <row r="1" ht="38.25" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F.I.SH</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Ta'lim yo'nalishi</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Passport</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Shartnoma raqam</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Viloyat</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tuman</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Telefon raqam</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Sana</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>15</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Amirov Akrom Eshali o'g'li</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>AC9990099</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>171</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Toʻraqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>06-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Amirov Akrom</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi 576 soat</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AA7777885</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>164</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Nurota tumani</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>24-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Amirov Akrom</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi 576 soat</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AA7777885</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>164</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Nurota tumani</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>24-10-2024</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
13:22 time 26.10.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -635,6 +635,90 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Amirov AKrom</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 864 soat</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>AA7777447</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>102</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Sirdaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Guliston shahri</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>+12676860109</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>26-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Amirov Akrom</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 864 soat</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>AA8888898</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Yangibozor tumani</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>+12676860109</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>26-10-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
8:53 time 03.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -719,6 +719,1686 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Amirov Akrom</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>AA1112233</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Toʻraqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>26-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Po'latova Shaxzoda Bekmirza qizi</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 576 soat</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>AD3798796</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>176</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Kosonsoy tumani</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>998907540390</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>27-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Abdujaparova Saodat Djeldoshevna</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>AD6108530</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>177</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>998994393636</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>27-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Fozilov Sobir Savriyech</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>AB6413136</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>177</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Shofirkon tumani</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>998932218088</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>27-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Nig'matjonova Saodat Abduraxim qizi</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>AD5364679</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>178</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>998997979464</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>29-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Abdujaparova Saodat Djeldoshevna</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>AD6108530</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>179</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>998994393636</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>29-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sheraliyeva Soraxon</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti psixologi</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>AD6836527</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Xoʻjaobod tumani</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>998905719115</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>30-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Rozimetova Guzal Ruslanovna</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>AD3394674</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>181</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>998900072962</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Toirova Shaxnoza Kaxramanovna</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>AD1148433</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>182</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>998946403222</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Siddikova Zulfiya Qobul qizi</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>AD6989709</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>183</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>998946897470</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Djurayeva Lazokat Azizovna</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>AB0542827</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>184</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>998909280026</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Djurayeva Dilnoza Gayratjanovna</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>AD7613232</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>185</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>998930903544</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Inogamova Nazokat Miradilovna</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>AD8944605</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>186</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>998994440012</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Mirxamidova Munisa Rustamovna</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>AD3841403</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>998998393917</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Axmedova Zarina Boltabayevna</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>AB3219478</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Buxoro tumani</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>998907186900</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Rasulova Munojot Tohirovna</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>AD6434587</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Romitan tumani</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>998995847437</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Xudayberdiyeva Gulsara Chuyanovna</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi 576 soat</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>AB4316277</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Qarshi tumani</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>998907214410</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Barotova Aziza Siroj qizi</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>AD2911314</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Buxoro tumani</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>998973033346</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Alijanova Gulchehra Ganijanovna</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>AD7140637</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>191</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Namangan tumani</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>998913687179</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ergasheva Mamlakat Mahmudovna</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>AC0347165</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>192</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Namangan tumani</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>998905996750</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Sadikova Dildorxon Muhammadjonovna</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>AD0511160</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>193</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Fargʻona tumani</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>998905357100</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Umarova Kamola Xabibullayevna</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>AD1955304</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>998903280500</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Sagdiyeva Lobar Muhamatovna</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>AD5447896</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>998946978186</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Hazratova Laylo Azamovna</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>AB6461603</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>196</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Romitan tumani</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>998993507334</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Toshpulatova Nilufar Turakulovna</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>AB5932070</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>998904511441</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Ergasheva Muqaddam Mahmudovna</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>AB9794964</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>198</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Namangan tumani</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>998905544944</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Jakbarova Malika Nematullayevna</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>AC0704078</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>199</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Uychi tumani</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>998939142560</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Raximova Dilafruz Solejonovna</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>AB1980507</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>998937269259</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Abdullayeva Maston Nazarbayevna</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>AC0329323</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Namangan tumani</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>998913524944</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Yusubova Moxchehra Abdivaydulayevna</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>AA9113347</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>202</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>998915490785</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Abduraximova Gulmira Olimjonovna</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>AB3073863</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Namangan tumani</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>998934062607</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Boboyeva Dilshoda Jumayevna</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>AC2379043</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>204</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Bekobod tumani</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>998943808012</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Izimbetova Bibinaz Sabitovna</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 864 soat</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>AD7875623</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Chimboy tumani</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>998904212177</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Azimova Anzirat Shoyiqulovna</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>AA6597541</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>206</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Romitan tumani</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>998932920601</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Bakhrieva Munira Erkinovna</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>AB6920673</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>998974053530</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Kurbanbaeva Dildora Kuralbay qizi</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>KA0802004</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>208</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Qoʻngʻirot tumani</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>998932149393</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Kurbanbaeva Dildora Kuralbay qizi</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 576 soat</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>KA0802014</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Qoʻngʻirot tumani</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>998932149393</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Ernazarova Munisa Ilg'or yo'lchi qizi</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>AD0534543</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>998770502921</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Baratova Gulmira Saidqulovna</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>AD2262661</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>998979100534</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Karshiboyeva Gulshan Furqatovna</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>AD8756217</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>998945335893</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12:31 time 03.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -2567,6 +2567,48 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Ashirboyeva Shoxsanam Shoikromovna</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>AD5815225</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>217</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>+998909794434</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>03-11-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12:57 time 03.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asosiy\Teloegram_bot_P\Nodavlat_MTT\file_service\file_database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bot\elbotwin\elbotr3\Nodavlat_MTT\file_service\file_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD38CA2-0021-4BB3-ABE5-8C5E61E3CB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="245">
   <si>
     <t>F.I.SH</t>
   </si>
@@ -746,12 +745,21 @@
   </si>
   <si>
     <t>998990634566</t>
+  </si>
+  <si>
+    <t>Ashirboyeva Shoxsanam Shoikromovna</t>
+  </si>
+  <si>
+    <t>AD5815225</t>
+  </si>
+  <si>
+    <t>217</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -797,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -808,6 +816,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1121,11 +1130,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:XFD51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2440,6 +2449,32 @@
         <v>227</v>
       </c>
     </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>242</v>
+      </c>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" t="s">
+        <v>243</v>
+      </c>
+      <c r="D51" t="s">
+        <v>244</v>
+      </c>
+      <c r="E51" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" t="s">
+        <v>85</v>
+      </c>
+      <c r="G51" s="4">
+        <v>998909794434</v>
+      </c>
+      <c r="H51" t="s">
+        <v>227</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
15:31 time 11.19.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A51" sqref="A51:XFD51"/>
@@ -3911,6 +3911,48 @@
         </is>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Jabborova Rano Rahmonovna</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>AD2380128</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>246</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>998972861919</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>13-11-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
15:11 time 22.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A51" sqref="A51:XFD51"/>
@@ -3953,6 +3953,238 @@
         </is>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Qosimova Nigoraxon Mahmudjon qizi</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>AB7943865</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>262</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>998990335588</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>20-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Dadaboyeva Marhabo G'aniyevna</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti psixologi</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>AB4871365</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>263</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>998994314929</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>20-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Jumaboyeva Mohiyaxon Ismoilovna</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>AD2021085</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>264</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>998999055045</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>20-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Yunusova Gulnoza Xikmatilla qizi</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>AB9919991</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>265</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Yuqori Chirchiq tumani</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>998943789199</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>20-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Soxibova Shaxodat Komilovna</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>AB0831483</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>266</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Uchqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>998974675009</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>20-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Maxammadiyeva Surayyo Normuradovna</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>AD7998828</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>267</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Navoiy shahri</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>998943799003</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>20-11-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
15:39 time 23.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A51" sqref="A51:XFD51"/>
@@ -4185,6 +4185,48 @@
         </is>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Sagatova Ziyodaxon Taxirovna</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>AD1426517</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>268</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Oʻrta Chirchiq tumani</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>998936160710</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>23-11-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
9:49 time 03.12.2024 date server
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H125"/>
+  <dimension ref="A1:H156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A91" sqref="A91:XFD91"/>
@@ -5697,6 +5697,1308 @@
         </is>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Ramatov Yangiboy Jumanazarovich</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti musiqa rahbari</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>AB2864318</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>301</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>998912784165</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Sadilloyeva Dilfuza Shuxratovna</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi 576 soat</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>AB1130811</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>302</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Kogon tumani</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>998995558780</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Babayeva Kamola Xusanovna</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi 576 soat</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>AB4404861</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>303</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Angren shahri</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>998931852007</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Sadilloyeva Dilfuza Shuxratovna</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>AB1130811</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>304</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Buxoro tumani</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>998995558780</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Jurayeva Raxima Habibullayevna</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>AD3610244</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>305</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Kosonsoy tumani</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>998951015074</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Yo'ldasheva Nilufar Ibrohimovna</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>AD8567923</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>306</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Andijon shahri</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>998916004616</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Botirova Zamira O'ralovna</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>AD8925197</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>307</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>998909281743</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Ravshanova Marjona Aminjonovna</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 576 soat</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>AB4649674</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>308</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>998906564240</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>29-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Guylmamedova Raisa Viktorovna</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 576 soat</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>AD6571021</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>309</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>998994805061</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>29-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Komilova Nodiraxon Mahmudjon qizi</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta`lim tashkiloti tashkilot oshpazi</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>AB5582671</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>310</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>998948893272</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>29-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Mirzamatova Zulxumor Umaraliyevna</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta`lim tashkiloti tashkilot oshpazi</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>AD4202739</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>311</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>998936322172</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>29-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Isakova Ozodaxon Tulashovna</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>AA9447846</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>312</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Mirzo Ulugʻbek tumani</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>998950150201</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>29-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Maxkamova Ra'no Sadikjanovna</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>AD7811878</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>313</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Yuqori Chirchiq tumani</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>+998944298109</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>30-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Usmanova Zulfiya Rustamovna</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>AD1510147</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>314</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Fargʻona tumani</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>998948364949</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>30-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Mutalipova Nargiza Zakirovna</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>AD8099504</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>315</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>+998944298109</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>30-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Mahmudova Aziza Mirzahamdamovna</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>AD7813109</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>316</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>998777011980</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>30-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Avazova Muxayyoxon Muzaffarjon qizi</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>AC1436252</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>317</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Pop tumani</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>998976228333</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>30-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Xayrullayeva Shohista Bekmirza qizi</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>AC0459728</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>318</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>Yangi Namangan</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>998949709559</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>01-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Nurullayeva Nodira Maxmudovna</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>AA8228491</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>319</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>Buxoro tumani</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>998997361179</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>YULDASHEVA DILDORAHON</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>AA9049494</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>320</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>Andijon shahri</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>998932594176</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Irgasheva Shalola Djabbarovna</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>AD1330938</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>321</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Samarqand shahri</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>998992912547</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Islomova Mahliyo Komil qizi</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti psixologi</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>AC0282022</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>322</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Sharof Rashidov tumani</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>998932918995</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Rasulova Nargiza Raximdjanovna</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>AD6566738</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>323</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>998909313092</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Bozorova Aziz Djuraqulovna</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>AB5048108</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>324</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Samarqand shahri</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>998915552375</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Ahmedova Muhabbatxon Xojiakbarxon qizi</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti psixologi</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>AD6646697</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>325</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Shayxontohur tumani</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>998950775055</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Urunova Dildora Sirojiddinovna</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>AD1866387</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>326</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Samarqand shahri</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>998982732145</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Xudoyberdiyeva Zarnigor Kobiljonovna</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti psixologi</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>AA9000453</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>327</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Samarqand tumani</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>998979271393</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Muhammadieva Shoira Holmuratovna</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>AD4160337</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>328</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Samarqand shahri</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>998933552525</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Ochilova Dildora Normamatovna</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti psixologi</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>AD4285763</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>329</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Qarshi tumani</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>998973146151</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Qodirova Dilorom Alivayevna</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>AA2991834</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>330</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>998908058073</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Karimova Bonu Nazirjon qizi</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>AB3171517</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>331</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>998958154892</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
10:12 time 10.12.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H156"/>
+  <dimension ref="A1:H172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A91" sqref="A91:XFD91"/>
@@ -6999,6 +6999,678 @@
         </is>
       </c>
     </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Aleksevnina Elvira Samigullayevna</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>AD1153885</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>332</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>998903296045</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Karimova Nigora Abdug'oppor qizi</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti defektolog/logopedi</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>AB1487410</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Fargʻona tumani</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>998911268606</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Nabiyeva Diyora Mahmud qizi</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>AA9586555</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>334</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>998773434046</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Yuldasheva ShaxodatAbdugani Qizi</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>AB3849334</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>335</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Yangi Namangan</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>998940084991</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Xolmatova Nazokat Abdurashidovna</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 576 soat</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>AD3224685</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>336</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Yangiyoʻl tumani</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>998944176679</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Qarshiyeva Nargiza</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>AA6933915</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>337</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Yakkabogʻ tumani</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>998933948706</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Jalolova Shahnoza  Nizomiddinovna</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>AB6670685</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>338</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>998917909191</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Normatova Zamira Latifovna</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>AD2136078</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>339</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Asaka tumani</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>998934122687</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>G'oyibova Dilshoda Hamroqulovna</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti metodisti</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>AD8546284</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>340</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Qorakoʻl tumani</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>998930820105</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Raxmonova Dilafruz Ochilovna</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>AB3464045</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>341</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Qorakoʻl tumani</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>998943280180</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Tadjiyeva Svetlana Aktyamovna</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>AD2327516</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>342</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>998948364949</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Normatova Zamiraxon Latifovna</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi 576 soat</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>AD2136078</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>343</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Asaka tumani</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>998934122687</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Mutalova Nasiba Ochilova</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>AB9594554</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>344</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Qorakoʻl tumani</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>998939689434</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Saliea GulnozaTursunbayvna</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>AB4918887</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>345</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>998916479256</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>06-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Saliea GulnozaTursunbayvna</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>AB4918887</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>346</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Olmazor tumani</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>998916479256</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>06-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Fofurova Dilrabo Ravshanbekovna</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>AD1844351</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>347</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>998998859987</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>06-12-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
14:12 time 10.12.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H172"/>
+  <dimension ref="A1:H174"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A91" sqref="A91:XFD91"/>
@@ -7671,6 +7671,90 @@
         </is>
       </c>
     </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Xasanova Ma'rifat Aminovna</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti direktori</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>AB3171624</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>348</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Kogon tumani</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>998978608883</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>10-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Xashimova Dilnaz Sabitxanovna</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>AB0959509</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>349</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>998909779885</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>10-12-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
16:48 time 10.12.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H174"/>
+  <dimension ref="A1:H175"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
       <selection activeCell="A91" sqref="A91:XFD91"/>
@@ -7755,6 +7755,48 @@
         </is>
       </c>
     </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>G'aybulloyeva Dildora Pulotovns</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Maktabgacha talim tashkiloti tarbiyachisi</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>AB9662266</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>350</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Qorovulbozor tumani</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>998997041379</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>10-12-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>